<commit_message>
Added uncertainty ranges on fitted Pc curve
</commit_message>
<xml_diff>
--- a/python/expdataHISUSSdrainage.xlsx
+++ b/python/expdataHISUSSdrainage.xlsx
@@ -1489,7 +1489,7 @@
         <v>0.01438890327779217</v>
       </c>
       <c r="D2">
-        <v>0.08254241773034748</v>
+        <v>0.08254241773034747</v>
       </c>
       <c r="E2">
         <v>0.2542670963104517</v>
@@ -1934,7 +1934,7 @@
         <v>3.07300192083071</v>
       </c>
       <c r="E28">
-        <v>0.2636857788883799</v>
+        <v>0.2636857788883801</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1951,7 +1951,7 @@
         <v>3.190185516633054</v>
       </c>
       <c r="E29">
-        <v>0.2622923939013571</v>
+        <v>0.2622923939013573</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2087,7 +2087,7 @@
         <v>3.382010058044334</v>
       </c>
       <c r="E37">
-        <v>0.2568295272038656</v>
+        <v>0.2568295272038659</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2104,7 +2104,7 @@
         <v>3.442511918370217</v>
       </c>
       <c r="E38">
-        <v>0.2576195235342628</v>
+        <v>0.257619523534263</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2121,7 +2121,7 @@
         <v>3.392517912689623</v>
       </c>
       <c r="E39">
-        <v>0.2540985319026466</v>
+        <v>0.2540985319026468</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2305,7 +2305,7 @@
         <v>0.6906673573340241</v>
       </c>
       <c r="D50">
-        <v>3.417877142298798</v>
+        <v>3.417877142298797</v>
       </c>
       <c r="E50">
         <v>0.2596690801590042</v>
@@ -2325,7 +2325,7 @@
         <v>3.494624435148761</v>
       </c>
       <c r="E51">
-        <v>0.2558097389024538</v>
+        <v>0.255809738902454</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2478,7 +2478,7 @@
         <v>3.441782369245478</v>
       </c>
       <c r="E60">
-        <v>0.2595775485727188</v>
+        <v>0.2595775485727185</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2611,10 +2611,10 @@
         <v>0.9496676163342832</v>
       </c>
       <c r="D68">
-        <v>3.406887066150269</v>
+        <v>3.406887066150268</v>
       </c>
       <c r="E68">
-        <v>0.2580893224012585</v>
+        <v>0.2580893224012583</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2784,7 +2784,7 @@
         <v>3.842609546293314</v>
       </c>
       <c r="E78">
-        <v>0.2849649475790816</v>
+        <v>0.2849649475790814</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3070,10 +3070,10 @@
         <v>2.123802123802125</v>
       </c>
       <c r="D95">
-        <v>5.028257205327956</v>
+        <v>5.028257205327963</v>
       </c>
       <c r="E95">
-        <v>0.4267124367158776</v>
+        <v>0.4267124367158778</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3087,7 +3087,7 @@
         <v>2.267691156580045</v>
       </c>
       <c r="D96">
-        <v>5.102329099432594</v>
+        <v>5.102329099432601</v>
       </c>
       <c r="E96">
         <v>0.4239147421577732</v>
@@ -3104,10 +3104,10 @@
         <v>2.411580189357968</v>
       </c>
       <c r="D97">
-        <v>5.244997656220224</v>
+        <v>5.244997656220231</v>
       </c>
       <c r="E97">
-        <v>0.4167843247288421</v>
+        <v>0.4167843247288424</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -3121,7 +3121,7 @@
         <v>2.555469222135889</v>
       </c>
       <c r="D98">
-        <v>5.220991114447282</v>
+        <v>5.220991114447289</v>
       </c>
       <c r="E98">
         <v>0.4109033427473405</v>
@@ -3138,7 +3138,7 @@
         <v>2.699358254913812</v>
       </c>
       <c r="D99">
-        <v>5.257609950949671</v>
+        <v>5.257609950949679</v>
       </c>
       <c r="E99">
         <v>0.4121647826100899</v>
@@ -3155,7 +3155,7 @@
         <v>2.843247287691733</v>
       </c>
       <c r="D100">
-        <v>5.290491240323516</v>
+        <v>5.290491240323523</v>
       </c>
       <c r="E100">
         <v>0.4071017957703045</v>
@@ -3172,7 +3172,7 @@
         <v>2.987136320469654</v>
       </c>
       <c r="D101">
-        <v>5.366593308627812</v>
+        <v>5.366593308627819</v>
       </c>
       <c r="E101">
         <v>0.4107846793021018</v>
@@ -3189,7 +3189,7 @@
         <v>3.131025353247577</v>
       </c>
       <c r="D102">
-        <v>5.325569223124985</v>
+        <v>5.325569223124992</v>
       </c>
       <c r="E102">
         <v>0.4128497546008257</v>
@@ -3206,7 +3206,7 @@
         <v>3.274914386025498</v>
       </c>
       <c r="D103">
-        <v>5.348738289336204</v>
+        <v>5.348738289336211</v>
       </c>
       <c r="E103">
         <v>0.4106562365008418</v>
@@ -3223,7 +3223,7 @@
         <v>3.418803418803419</v>
       </c>
       <c r="D104">
-        <v>5.355618311065706</v>
+        <v>5.355618311065713</v>
       </c>
       <c r="E104">
         <v>0.4088362742154091</v>
@@ -3532,10 +3532,10 @@
         <v>0.5058296888071141</v>
       </c>
       <c r="M2">
-        <v>0.5095515274443498</v>
+        <v>0.5095515274443497</v>
       </c>
       <c r="N2">
-        <v>0.4881232612425518</v>
+        <v>0.488123261242552</v>
       </c>
       <c r="O2">
         <v>0.4874173021001929</v>
@@ -3600,7 +3600,7 @@
         <v>0.5090385053498641</v>
       </c>
       <c r="L3">
-        <v>0.4999807309750827</v>
+        <v>0.4999807309750828</v>
       </c>
       <c r="M3">
         <v>0.5086578496023169</v>
@@ -3618,16 +3618,16 @@
         <v>0.4157599122246941</v>
       </c>
       <c r="R3">
-        <v>0.3674683642266039</v>
+        <v>0.3674683642266038</v>
       </c>
       <c r="S3">
-        <v>0.3386045826884461</v>
+        <v>0.338604582688446</v>
       </c>
       <c r="T3">
         <v>0.3214638075468391</v>
       </c>
       <c r="U3">
-        <v>0.3358205351992548</v>
+        <v>0.3358205351992549</v>
       </c>
       <c r="V3">
         <v>0.2849677832858031</v>
@@ -3677,7 +3677,7 @@
         <v>0.5104603922301844</v>
       </c>
       <c r="N4">
-        <v>0.4859106803985623</v>
+        <v>0.4859106803985624</v>
       </c>
       <c r="O4">
         <v>0.4906805785101743</v>
@@ -3686,10 +3686,10 @@
         <v>0.4691613511150506</v>
       </c>
       <c r="Q4">
-        <v>0.4333005777329978</v>
+        <v>0.4333005777329976</v>
       </c>
       <c r="R4">
-        <v>0.376935353082745</v>
+        <v>0.3769353530827448</v>
       </c>
       <c r="S4">
         <v>0.345086199549283</v>
@@ -3698,7 +3698,7 @@
         <v>0.3382522752234439</v>
       </c>
       <c r="U4">
-        <v>0.3339858863836895</v>
+        <v>0.3339858863836896</v>
       </c>
       <c r="V4">
         <v>0.2622945312211599</v>
@@ -3742,25 +3742,25 @@
         <v>0.519531725417941</v>
       </c>
       <c r="L5">
-        <v>0.5241096014777131</v>
+        <v>0.5241096014777129</v>
       </c>
       <c r="M5">
         <v>0.4995955693581263</v>
       </c>
       <c r="N5">
-        <v>0.5072042038291587</v>
+        <v>0.5072042038291588</v>
       </c>
       <c r="O5">
         <v>0.4896895544577962</v>
       </c>
       <c r="P5">
-        <v>0.4603372468768088</v>
+        <v>0.4603372468768089</v>
       </c>
       <c r="Q5">
-        <v>0.4238493581627719</v>
+        <v>0.4238493581627718</v>
       </c>
       <c r="R5">
-        <v>0.3989456003308133</v>
+        <v>0.3989456003308134</v>
       </c>
       <c r="S5">
         <v>0.3390892657305376</v>
@@ -3816,13 +3816,13 @@
         <v>0.5108234150336783</v>
       </c>
       <c r="M6">
-        <v>0.4889713514807412</v>
+        <v>0.488971351480741</v>
       </c>
       <c r="N6">
         <v>0.5010753757388935</v>
       </c>
       <c r="O6">
-        <v>0.4833123697895974</v>
+        <v>0.4833123697895972</v>
       </c>
       <c r="P6">
         <v>0.4478672471548628</v>
@@ -3840,7 +3840,7 @@
         <v>0.3222386631996108</v>
       </c>
       <c r="U6">
-        <v>0.3338705783334177</v>
+        <v>0.3338705783334178</v>
       </c>
       <c r="V6">
         <v>0.2838889991895931</v>
@@ -3890,28 +3890,28 @@
         <v>0.4990525714193289</v>
       </c>
       <c r="N7">
-        <v>0.5069920130786044</v>
+        <v>0.5069920130786043</v>
       </c>
       <c r="O7">
         <v>0.4964340503195737</v>
       </c>
       <c r="P7">
-        <v>0.4619310611116234</v>
+        <v>0.4619310611116231</v>
       </c>
       <c r="Q7">
         <v>0.4343967513375095</v>
       </c>
       <c r="R7">
-        <v>0.3830298429210879</v>
+        <v>0.3830298429210878</v>
       </c>
       <c r="S7">
-        <v>0.3420984119784464</v>
+        <v>0.3420984119784465</v>
       </c>
       <c r="T7">
         <v>0.3413016531459568</v>
       </c>
       <c r="U7">
-        <v>0.339521321141598</v>
+        <v>0.3395213211415979</v>
       </c>
       <c r="V7">
         <v>0.2632469189152534</v>
@@ -3955,7 +3955,7 @@
         <v>0.5428419852020776</v>
       </c>
       <c r="L8">
-        <v>0.5129450256548533</v>
+        <v>0.5129450256548534</v>
       </c>
       <c r="M8">
         <v>0.5193878979667433</v>
@@ -3967,19 +3967,19 @@
         <v>0.5012100667579619</v>
       </c>
       <c r="P8">
-        <v>0.4644505868042623</v>
+        <v>0.4644505868042624</v>
       </c>
       <c r="Q8">
         <v>0.4309207199204552</v>
       </c>
       <c r="R8">
-        <v>0.3949387187845736</v>
+        <v>0.3949387187845737</v>
       </c>
       <c r="S8">
-        <v>0.3336617693339436</v>
+        <v>0.3336617693339435</v>
       </c>
       <c r="T8">
-        <v>0.3234850482554617</v>
+        <v>0.3234850482554618</v>
       </c>
       <c r="U8">
         <v>0.3270984260115353</v>
@@ -4041,13 +4041,13 @@
         <v>0.4610701332711117</v>
       </c>
       <c r="Q9">
-        <v>0.4239964182075904</v>
+        <v>0.4239964182075903</v>
       </c>
       <c r="R9">
-        <v>0.3995939691084255</v>
+        <v>0.3995939691084254</v>
       </c>
       <c r="S9">
-        <v>0.3392980685124492</v>
+        <v>0.3392980685124493</v>
       </c>
       <c r="T9">
         <v>0.3458513891154414</v>
@@ -4109,22 +4109,22 @@
         <v>0.5169150095994345</v>
       </c>
       <c r="P10">
-        <v>0.4828319758605246</v>
+        <v>0.4828319758605248</v>
       </c>
       <c r="Q10">
         <v>0.4245389609415309</v>
       </c>
       <c r="R10">
-        <v>0.3988274092094269</v>
+        <v>0.3988274092094268</v>
       </c>
       <c r="S10">
         <v>0.3497638793617186</v>
       </c>
       <c r="T10">
-        <v>0.3454883887954329</v>
+        <v>0.345488388795433</v>
       </c>
       <c r="U10">
-        <v>0.3526964399747267</v>
+        <v>0.3526964399747268</v>
       </c>
       <c r="V10">
         <v>0.2786443982267771</v>
@@ -4168,7 +4168,7 @@
         <v>0.535981381053226</v>
       </c>
       <c r="L11">
-        <v>0.5252226256267718</v>
+        <v>0.5252226256267717</v>
       </c>
       <c r="M11">
         <v>0.5100007096878773</v>
@@ -4180,19 +4180,19 @@
         <v>0.5095634418173829</v>
       </c>
       <c r="P11">
-        <v>0.4697508563613327</v>
+        <v>0.4697508563613326</v>
       </c>
       <c r="Q11">
-        <v>0.4439256890765942</v>
+        <v>0.4439256890765944</v>
       </c>
       <c r="R11">
-        <v>0.3998326220348744</v>
+        <v>0.3998326220348745</v>
       </c>
       <c r="S11">
-        <v>0.3524313377228373</v>
+        <v>0.3524313377228374</v>
       </c>
       <c r="T11">
-        <v>0.3524682699516114</v>
+        <v>0.3524682699516115</v>
       </c>
       <c r="U11">
         <v>0.354620062854688</v>
@@ -4239,10 +4239,10 @@
         <v>0.5582712744125093</v>
       </c>
       <c r="L12">
-        <v>0.5241799691341955</v>
+        <v>0.5241799691341954</v>
       </c>
       <c r="M12">
-        <v>0.5208239007242214</v>
+        <v>0.5208239007242215</v>
       </c>
       <c r="N12">
         <v>0.5131594697726167</v>
@@ -4254,16 +4254,16 @@
         <v>0.4938345773634271</v>
       </c>
       <c r="Q12">
-        <v>0.4304245581140615</v>
+        <v>0.4304245581140613</v>
       </c>
       <c r="R12">
-        <v>0.4050542483990868</v>
+        <v>0.4050542483990869</v>
       </c>
       <c r="S12">
-        <v>0.3703326823550619</v>
+        <v>0.3703326823550618</v>
       </c>
       <c r="T12">
-        <v>0.3458872111528429</v>
+        <v>0.345887211152843</v>
       </c>
       <c r="U12">
         <v>0.3495694304947202</v>
@@ -4310,10 +4310,10 @@
         <v>0.56810570668272</v>
       </c>
       <c r="L13">
-        <v>0.5469236111569769</v>
+        <v>0.546923611156977</v>
       </c>
       <c r="M13">
-        <v>0.5209143893503246</v>
+        <v>0.5209143893503244</v>
       </c>
       <c r="N13">
         <v>0.5255029107154962</v>
@@ -4393,10 +4393,10 @@
         <v>0.5210630178247617</v>
       </c>
       <c r="P14">
-        <v>0.4780725114413846</v>
+        <v>0.4780725114413847</v>
       </c>
       <c r="Q14">
-        <v>0.4411779137524151</v>
+        <v>0.441177913752415</v>
       </c>
       <c r="R14">
         <v>0.4090552357938025</v>
@@ -4405,10 +4405,10 @@
         <v>0.3504327250822666</v>
       </c>
       <c r="T14">
-        <v>0.3580655000093438</v>
+        <v>0.3580655000093437</v>
       </c>
       <c r="U14">
-        <v>0.3639690286989629</v>
+        <v>0.3639690286989628</v>
       </c>
       <c r="V14">
         <v>0.3008723852941912</v>
@@ -4452,7 +4452,7 @@
         <v>0.5713480245694826</v>
       </c>
       <c r="L15">
-        <v>0.5472957096051404</v>
+        <v>0.5472957096051403</v>
       </c>
       <c r="M15">
         <v>0.5264001454791515</v>
@@ -4461,19 +4461,19 @@
         <v>0.5105068762355256</v>
       </c>
       <c r="O15">
-        <v>0.521145091017968</v>
+        <v>0.5211450910179681</v>
       </c>
       <c r="P15">
         <v>0.4995986593586371</v>
       </c>
       <c r="Q15">
-        <v>0.4686202111512067</v>
+        <v>0.4686202111512068</v>
       </c>
       <c r="R15">
-        <v>0.4129918792348222</v>
+        <v>0.4129918792348221</v>
       </c>
       <c r="S15">
-        <v>0.3657957137043451</v>
+        <v>0.3657957137043453</v>
       </c>
       <c r="T15">
         <v>0.3403883320723147</v>
@@ -4523,34 +4523,34 @@
         <v>0.5749885719466398</v>
       </c>
       <c r="L16">
-        <v>0.5636949705307517</v>
+        <v>0.5636949705307519</v>
       </c>
       <c r="M16">
         <v>0.5249021547998876</v>
       </c>
       <c r="N16">
-        <v>0.5135957548572058</v>
+        <v>0.5135957548572059</v>
       </c>
       <c r="O16">
-        <v>0.5316477115419486</v>
+        <v>0.5316477115419487</v>
       </c>
       <c r="P16">
-        <v>0.5024969811193233</v>
+        <v>0.5024969811193232</v>
       </c>
       <c r="Q16">
-        <v>0.4515989035802733</v>
+        <v>0.4515989035802734</v>
       </c>
       <c r="R16">
         <v>0.4181541119603467</v>
       </c>
       <c r="S16">
-        <v>0.3762438004300266</v>
+        <v>0.3762438004300265</v>
       </c>
       <c r="T16">
         <v>0.3576014363784861</v>
       </c>
       <c r="U16">
-        <v>0.3539365951771588</v>
+        <v>0.3539365951771589</v>
       </c>
       <c r="V16">
         <v>0.3068800266727268</v>
@@ -4600,7 +4600,7 @@
         <v>0.5259994489706815</v>
       </c>
       <c r="N17">
-        <v>0.5277525185143511</v>
+        <v>0.527752518514351</v>
       </c>
       <c r="O17">
         <v>0.5433621504285774</v>
@@ -4609,7 +4609,7 @@
         <v>0.5030008270823261</v>
       </c>
       <c r="Q17">
-        <v>0.4738041378649476</v>
+        <v>0.4738041378649475</v>
       </c>
       <c r="R17">
         <v>0.4450496984976238</v>
@@ -4665,7 +4665,7 @@
         <v>0.5625297640189013</v>
       </c>
       <c r="L18">
-        <v>0.5663217108230431</v>
+        <v>0.5663217108230432</v>
       </c>
       <c r="M18">
         <v>0.5297998725492986</v>
@@ -4674,19 +4674,19 @@
         <v>0.5301118420308949</v>
       </c>
       <c r="O18">
-        <v>0.5225265480646175</v>
+        <v>0.5225265480646176</v>
       </c>
       <c r="P18">
-        <v>0.5109125635113422</v>
+        <v>0.5109125635113423</v>
       </c>
       <c r="Q18">
         <v>0.4685178502188274</v>
       </c>
       <c r="R18">
-        <v>0.4473700782602443</v>
+        <v>0.4473700782602442</v>
       </c>
       <c r="S18">
-        <v>0.3879318846968317</v>
+        <v>0.3879318846968315</v>
       </c>
       <c r="T18">
         <v>0.3761862213563713</v>
@@ -4742,13 +4742,13 @@
         <v>0.5283578870091015</v>
       </c>
       <c r="N19">
-        <v>0.5484982331978292</v>
+        <v>0.5484982331978291</v>
       </c>
       <c r="O19">
-        <v>0.5424251081816087</v>
+        <v>0.5424251081816085</v>
       </c>
       <c r="P19">
-        <v>0.5232996387029624</v>
+        <v>0.5232996387029625</v>
       </c>
       <c r="Q19">
         <v>0.4556753608177075</v>
@@ -4757,13 +4757,13 @@
         <v>0.4544015438125766</v>
       </c>
       <c r="S19">
-        <v>0.3648990913122172</v>
+        <v>0.3648990913122173</v>
       </c>
       <c r="T19">
         <v>0.3688447745493</v>
       </c>
       <c r="U19">
-        <v>0.3674089829849768</v>
+        <v>0.3674089829849767</v>
       </c>
       <c r="V19">
         <v>0.3152494021756672</v>
@@ -4807,25 +4807,25 @@
         <v>0.5955339140284163</v>
       </c>
       <c r="L20">
-        <v>0.5563511452293135</v>
+        <v>0.5563511452293134</v>
       </c>
       <c r="M20">
-        <v>0.5599650586684572</v>
+        <v>0.5599650586684574</v>
       </c>
       <c r="N20">
-        <v>0.5280706276314899</v>
+        <v>0.5280706276314898</v>
       </c>
       <c r="O20">
         <v>0.536758730809172</v>
       </c>
       <c r="P20">
-        <v>0.5229809480925763</v>
+        <v>0.5229809480925762</v>
       </c>
       <c r="Q20">
-        <v>0.4645081921380406</v>
+        <v>0.4645081921380405</v>
       </c>
       <c r="R20">
-        <v>0.4581522386491728</v>
+        <v>0.4581522386491727</v>
       </c>
       <c r="S20">
         <v>0.3900340807753316</v>
@@ -4878,10 +4878,10 @@
         <v>0.603075367688459</v>
       </c>
       <c r="L21">
-        <v>0.5609135732613978</v>
+        <v>0.5609135732613979</v>
       </c>
       <c r="M21">
-        <v>0.5641022239366241</v>
+        <v>0.5641022239366242</v>
       </c>
       <c r="N21">
         <v>0.5488749801336901</v>
@@ -4893,22 +4893,22 @@
         <v>0.5238917443530511</v>
       </c>
       <c r="Q21">
-        <v>0.4727052721494341</v>
+        <v>0.472705272149434</v>
       </c>
       <c r="R21">
         <v>0.4353892289341297</v>
       </c>
       <c r="S21">
-        <v>0.3798453015483329</v>
+        <v>0.379845301548333</v>
       </c>
       <c r="T21">
         <v>0.3667509475184871</v>
       </c>
       <c r="U21">
-        <v>0.3692855391456817</v>
+        <v>0.3692855391456815</v>
       </c>
       <c r="V21">
-        <v>0.3036569566586655</v>
+        <v>0.3036569566586654</v>
       </c>
       <c r="W21">
         <v>0.3142436901140663</v>
@@ -4952,16 +4952,16 @@
         <v>0.5910420692121271</v>
       </c>
       <c r="M22">
-        <v>0.5417571747844326</v>
+        <v>0.5417571747844327</v>
       </c>
       <c r="N22">
-        <v>0.5598551963418713</v>
+        <v>0.5598551963418712</v>
       </c>
       <c r="O22">
         <v>0.5399519329493462</v>
       </c>
       <c r="P22">
-        <v>0.5216171294506831</v>
+        <v>0.5216171294506829</v>
       </c>
       <c r="Q22">
         <v>0.4777278432983723</v>
@@ -4979,7 +4979,7 @@
         <v>0.3790639265358187</v>
       </c>
       <c r="V22">
-        <v>0.3099725687622576</v>
+        <v>0.3099725687622577</v>
       </c>
       <c r="W22">
         <v>0.3102621330098502</v>
@@ -5035,7 +5035,7 @@
         <v>0.5204355704707341</v>
       </c>
       <c r="Q23">
-        <v>0.4864632505043778</v>
+        <v>0.4864632505043779</v>
       </c>
       <c r="R23">
         <v>0.4527897782307325</v>
@@ -5044,13 +5044,13 @@
         <v>0.3989024124091067</v>
       </c>
       <c r="T23">
-        <v>0.383711861229129</v>
+        <v>0.3837118612291289</v>
       </c>
       <c r="U23">
         <v>0.3931140182876962</v>
       </c>
       <c r="V23">
-        <v>0.3179534825835641</v>
+        <v>0.3179534825835642</v>
       </c>
       <c r="W23">
         <v>0.3284822120904754</v>
@@ -5091,31 +5091,31 @@
         <v>0.5987231944470827</v>
       </c>
       <c r="L24">
-        <v>0.5864954030740983</v>
+        <v>0.5864954030740982</v>
       </c>
       <c r="M24">
         <v>0.5596224375946505</v>
       </c>
       <c r="N24">
-        <v>0.5669418633235138</v>
+        <v>0.5669418633235137</v>
       </c>
       <c r="O24">
-        <v>0.5427863833975536</v>
+        <v>0.5427863833975537</v>
       </c>
       <c r="P24">
-        <v>0.523912847449948</v>
+        <v>0.5239128474499481</v>
       </c>
       <c r="Q24">
-        <v>0.4918790448838144</v>
+        <v>0.4918790448838145</v>
       </c>
       <c r="R24">
-        <v>0.4716308693755015</v>
+        <v>0.4716308693755016</v>
       </c>
       <c r="S24">
         <v>0.4122768059574201</v>
       </c>
       <c r="T24">
-        <v>0.3825981483628048</v>
+        <v>0.3825981483628049</v>
       </c>
       <c r="U24">
         <v>0.38365374978228</v>
@@ -5168,7 +5168,7 @@
         <v>0.5746426970393983</v>
       </c>
       <c r="N25">
-        <v>0.5484245321947957</v>
+        <v>0.5484245321947956</v>
       </c>
       <c r="O25">
         <v>0.5574404077236789</v>
@@ -5177,19 +5177,19 @@
         <v>0.5290976603425913</v>
       </c>
       <c r="Q25">
-        <v>0.487768742289554</v>
+        <v>0.4877687422895541</v>
       </c>
       <c r="R25">
-        <v>0.4804125909572216</v>
+        <v>0.4804125909572217</v>
       </c>
       <c r="S25">
         <v>0.3917029955414621</v>
       </c>
       <c r="T25">
-        <v>0.3868498876855128</v>
+        <v>0.3868498876855129</v>
       </c>
       <c r="U25">
-        <v>0.378505142277025</v>
+        <v>0.3785051422770249</v>
       </c>
       <c r="V25">
         <v>0.336137799609545</v>
@@ -5236,22 +5236,22 @@
         <v>0.5974162782051855</v>
       </c>
       <c r="M26">
-        <v>0.5810318826123301</v>
+        <v>0.5810318826123302</v>
       </c>
       <c r="N26">
-        <v>0.5516582895741422</v>
+        <v>0.5516582895741424</v>
       </c>
       <c r="O26">
         <v>0.5659373345856796</v>
       </c>
       <c r="P26">
-        <v>0.5539353008241376</v>
+        <v>0.5539353008241374</v>
       </c>
       <c r="Q26">
         <v>0.4857624652340009</v>
       </c>
       <c r="R26">
-        <v>0.4778618164404828</v>
+        <v>0.4778618164404826</v>
       </c>
       <c r="S26">
         <v>0.4087171572973599</v>
@@ -5260,7 +5260,7 @@
         <v>0.3861059512808364</v>
       </c>
       <c r="U26">
-        <v>0.3899550402469254</v>
+        <v>0.3899550402469255</v>
       </c>
       <c r="V26">
         <v>0.3256890744675325</v>
@@ -5307,7 +5307,7 @@
         <v>0.6106195288471239</v>
       </c>
       <c r="M27">
-        <v>0.5609209263009859</v>
+        <v>0.560920926300986</v>
       </c>
       <c r="N27">
         <v>0.5602033200026489</v>
@@ -5316,7 +5316,7 @@
         <v>0.5610632600990966</v>
       </c>
       <c r="P27">
-        <v>0.5361139777634385</v>
+        <v>0.5361139777634384</v>
       </c>
       <c r="Q27">
         <v>0.5093054200746983</v>
@@ -5381,22 +5381,22 @@
         <v>0.5738089910688595</v>
       </c>
       <c r="N28">
-        <v>0.5738536061180163</v>
+        <v>0.5738536061180162</v>
       </c>
       <c r="O28">
         <v>0.5712134742227218</v>
       </c>
       <c r="P28">
-        <v>0.5412509663910555</v>
+        <v>0.5412509663910556</v>
       </c>
       <c r="Q28">
         <v>0.5075125058120014</v>
       </c>
       <c r="R28">
-        <v>0.4834231207885711</v>
+        <v>0.4834231207885712</v>
       </c>
       <c r="S28">
-        <v>0.4303244250821319</v>
+        <v>0.4303244250821318</v>
       </c>
       <c r="T28">
         <v>0.4175990011818408</v>
@@ -5452,28 +5452,28 @@
         <v>0.5865909889012448</v>
       </c>
       <c r="N29">
-        <v>0.582705936061764</v>
+        <v>0.5827059360617641</v>
       </c>
       <c r="O29">
         <v>0.5767766167708297</v>
       </c>
       <c r="P29">
-        <v>0.5437850382486631</v>
+        <v>0.543785038248663</v>
       </c>
       <c r="Q29">
         <v>0.5197822043316592</v>
       </c>
       <c r="R29">
-        <v>0.487766311193842</v>
+        <v>0.4877663111938421</v>
       </c>
       <c r="S29">
-        <v>0.4096037607474486</v>
+        <v>0.4096037607474488</v>
       </c>
       <c r="T29">
-        <v>0.4196935738888765</v>
+        <v>0.4196935738888763</v>
       </c>
       <c r="U29">
-        <v>0.4034327278477527</v>
+        <v>0.4034327278477529</v>
       </c>
       <c r="V29">
         <v>0.3415775295329554</v>
@@ -5526,25 +5526,25 @@
         <v>0.591770402875585</v>
       </c>
       <c r="O30">
-        <v>0.5877700803084057</v>
+        <v>0.5877700803084056</v>
       </c>
       <c r="P30">
-        <v>0.5711424116601461</v>
+        <v>0.5711424116601462</v>
       </c>
       <c r="Q30">
         <v>0.5219505569992816</v>
       </c>
       <c r="R30">
-        <v>0.5064540994335127</v>
+        <v>0.5064540994335128</v>
       </c>
       <c r="S30">
-        <v>0.4392981482042166</v>
+        <v>0.4392981482042167</v>
       </c>
       <c r="T30">
         <v>0.4164040098919242</v>
       </c>
       <c r="U30">
-        <v>0.431221216306993</v>
+        <v>0.4312212163069931</v>
       </c>
       <c r="V30">
         <v>0.3392875267396261</v>
@@ -5594,13 +5594,13 @@
         <v>0.6106962466869821</v>
       </c>
       <c r="N31">
-        <v>0.5970956376508187</v>
+        <v>0.5970956376508189</v>
       </c>
       <c r="O31">
         <v>0.5908990794656406</v>
       </c>
       <c r="P31">
-        <v>0.5548516616856483</v>
+        <v>0.5548516616856481</v>
       </c>
       <c r="Q31">
         <v>0.5106632699600402</v>
@@ -5609,19 +5609,19 @@
         <v>0.4963073202067799</v>
       </c>
       <c r="S31">
-        <v>0.435564021793719</v>
+        <v>0.4355640217937189</v>
       </c>
       <c r="T31">
-        <v>0.4329741381516455</v>
+        <v>0.4329741381516454</v>
       </c>
       <c r="U31">
         <v>0.4196278613079851</v>
       </c>
       <c r="V31">
-        <v>0.3629749655550106</v>
+        <v>0.3629749655550107</v>
       </c>
       <c r="W31">
-        <v>0.3611617181119257</v>
+        <v>0.3611617181119256</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -5674,25 +5674,25 @@
         <v>0.5891572576837405</v>
       </c>
       <c r="Q32">
-        <v>0.5414718277220356</v>
+        <v>0.5414718277220358</v>
       </c>
       <c r="R32">
         <v>0.4923801586527672</v>
       </c>
       <c r="S32">
-        <v>0.4548916470551173</v>
+        <v>0.4548916470551172</v>
       </c>
       <c r="T32">
-        <v>0.4202880898095367</v>
+        <v>0.4202880898095368</v>
       </c>
       <c r="U32">
-        <v>0.4309871481349356</v>
+        <v>0.4309871481349357</v>
       </c>
       <c r="V32">
         <v>0.3739966980272872</v>
       </c>
       <c r="W32">
-        <v>0.3591509924704344</v>
+        <v>0.3591509924704345</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -5730,19 +5730,19 @@
         <v>0.6520458308404715</v>
       </c>
       <c r="L33">
-        <v>0.6431437083912589</v>
+        <v>0.6431437083912588</v>
       </c>
       <c r="M33">
         <v>0.6089920800663429</v>
       </c>
       <c r="N33">
-        <v>0.6121869247979663</v>
+        <v>0.6121869247979664</v>
       </c>
       <c r="O33">
         <v>0.6009170750924868</v>
       </c>
       <c r="P33">
-        <v>0.5971884729355103</v>
+        <v>0.59718847293551</v>
       </c>
       <c r="Q33">
         <v>0.5470833618826039</v>
@@ -5751,10 +5751,10 @@
         <v>0.5026242826320412</v>
       </c>
       <c r="S33">
-        <v>0.4371583170585402</v>
+        <v>0.4371583170585404</v>
       </c>
       <c r="T33">
-        <v>0.429162280016454</v>
+        <v>0.4291622800164541</v>
       </c>
       <c r="U33">
         <v>0.4450601931651799</v>
@@ -5801,10 +5801,10 @@
         <v>0.6744050251694285</v>
       </c>
       <c r="L34">
-        <v>0.6321984732602325</v>
+        <v>0.6321984732602324</v>
       </c>
       <c r="M34">
-        <v>0.6023868780806282</v>
+        <v>0.6023868780806281</v>
       </c>
       <c r="N34">
         <v>0.5951322171371903</v>
@@ -5819,16 +5819,16 @@
         <v>0.5429123079641437</v>
       </c>
       <c r="R34">
-        <v>0.5237799287699562</v>
+        <v>0.5237799287699563</v>
       </c>
       <c r="S34">
-        <v>0.448488915344782</v>
+        <v>0.4484889153447819</v>
       </c>
       <c r="T34">
-        <v>0.448353666861831</v>
+        <v>0.4483536668618309</v>
       </c>
       <c r="U34">
-        <v>0.4304481873438276</v>
+        <v>0.4304481873438273</v>
       </c>
       <c r="V34">
         <v>0.3614023199419128</v>
@@ -5875,7 +5875,7 @@
         <v>0.6510105501093152</v>
       </c>
       <c r="M35">
-        <v>0.6161803363155628</v>
+        <v>0.6161803363155627</v>
       </c>
       <c r="N35">
         <v>0.6260602550476201</v>
@@ -5884,28 +5884,28 @@
         <v>0.6142017549867097</v>
       </c>
       <c r="P35">
-        <v>0.582519430359291</v>
+        <v>0.5825194303592911</v>
       </c>
       <c r="Q35">
-        <v>0.5620366419511192</v>
+        <v>0.5620366419511194</v>
       </c>
       <c r="R35">
         <v>0.5228948139977169</v>
       </c>
       <c r="S35">
-        <v>0.4644297528101989</v>
+        <v>0.4644297528101988</v>
       </c>
       <c r="T35">
-        <v>0.4415094637563594</v>
+        <v>0.4415094637563592</v>
       </c>
       <c r="U35">
-        <v>0.4499328251574954</v>
+        <v>0.4499328251574953</v>
       </c>
       <c r="V35">
         <v>0.3660032228595796</v>
       </c>
       <c r="W35">
-        <v>0.3759125040561449</v>
+        <v>0.3759125040561448</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -5946,10 +5946,10 @@
         <v>0.6632569211443361</v>
       </c>
       <c r="M36">
-        <v>0.6166996417415191</v>
+        <v>0.6166996417415193</v>
       </c>
       <c r="N36">
-        <v>0.6350916725261403</v>
+        <v>0.6350916725261402</v>
       </c>
       <c r="O36">
         <v>0.6156885130871208</v>
@@ -5970,10 +5970,10 @@
         <v>0.4675913548295834</v>
       </c>
       <c r="U36">
-        <v>0.4583399388434585</v>
+        <v>0.4583399388434586</v>
       </c>
       <c r="V36">
-        <v>0.3900877259839652</v>
+        <v>0.3900877259839653</v>
       </c>
       <c r="W36">
         <v>0.3856322601007482</v>
@@ -6014,7 +6014,7 @@
         <v>0.7105775643949785</v>
       </c>
       <c r="L37">
-        <v>0.6687875193006947</v>
+        <v>0.6687875193006948</v>
       </c>
       <c r="M37">
         <v>0.6486068899665788</v>
@@ -6026,13 +6026,13 @@
         <v>0.6177493434361723</v>
       </c>
       <c r="P37">
-        <v>0.6034026164624013</v>
+        <v>0.6034026164624012</v>
       </c>
       <c r="Q37">
         <v>0.5676387018948025</v>
       </c>
       <c r="R37">
-        <v>0.5433339271730812</v>
+        <v>0.5433339271730813</v>
       </c>
       <c r="S37">
         <v>0.4708273606774123</v>
@@ -6044,10 +6044,10 @@
         <v>0.4565935502075472</v>
       </c>
       <c r="V37">
-        <v>0.404832542639344</v>
+        <v>0.4048325426393441</v>
       </c>
       <c r="W37">
-        <v>0.4007909296901546</v>
+        <v>0.4007909296901545</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -6100,7 +6100,7 @@
         <v>0.6221335986575874</v>
       </c>
       <c r="Q38">
-        <v>0.576812286782693</v>
+        <v>0.5768122867826929</v>
       </c>
       <c r="R38">
         <v>0.5402890068989156</v>
@@ -6109,13 +6109,13 @@
         <v>0.4954813717711822</v>
       </c>
       <c r="T38">
-        <v>0.4941127341578576</v>
+        <v>0.4941127341578577</v>
       </c>
       <c r="U38">
-        <v>0.4872121532582643</v>
+        <v>0.4872121532582642</v>
       </c>
       <c r="V38">
-        <v>0.4195071401601895</v>
+        <v>0.4195071401601894</v>
       </c>
       <c r="W38">
         <v>0.4145447814626348</v>
@@ -6171,13 +6171,13 @@
         <v>0.6349721677443324</v>
       </c>
       <c r="Q39">
-        <v>0.5797688669262421</v>
+        <v>0.579768866926242</v>
       </c>
       <c r="R39">
         <v>0.5665931594664494</v>
       </c>
       <c r="S39">
-        <v>0.5010961199055172</v>
+        <v>0.5010961199055171</v>
       </c>
       <c r="T39">
         <v>0.4971011090654105</v>
@@ -6189,7 +6189,7 @@
         <v>0.4047617986191948</v>
       </c>
       <c r="W39">
-        <v>0.421210917717858</v>
+        <v>0.4212109177178581</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -6233,7 +6233,7 @@
         <v>0.6579831681152839</v>
       </c>
       <c r="N40">
-        <v>0.6571549263958322</v>
+        <v>0.6571549263958321</v>
       </c>
       <c r="O40">
         <v>0.656857776332615</v>
@@ -6316,7 +6316,7 @@
         <v>0.5981418602825328</v>
       </c>
       <c r="R41">
-        <v>0.5853449081778788</v>
+        <v>0.5853449081778789</v>
       </c>
       <c r="S41">
         <v>0.5350996235206009</v>
@@ -6325,7 +6325,7 @@
         <v>0.5204763540226551</v>
       </c>
       <c r="U41">
-        <v>0.516084708584562</v>
+        <v>0.5160847085845621</v>
       </c>
       <c r="V41">
         <v>0.4406237962603132</v>
@@ -6387,7 +6387,7 @@
         <v>0.6303157452074223</v>
       </c>
       <c r="R42">
-        <v>0.6104366461885007</v>
+        <v>0.6104366461885006</v>
       </c>
       <c r="S42">
         <v>0.5456285965671512</v>
@@ -6458,19 +6458,19 @@
         <v>0.6547352878501991</v>
       </c>
       <c r="R43">
-        <v>0.6289344356791085</v>
+        <v>0.6289344356791083</v>
       </c>
       <c r="S43">
         <v>0.5482712307598329</v>
       </c>
       <c r="T43">
-        <v>0.5379707689051912</v>
+        <v>0.5379707689051914</v>
       </c>
       <c r="U43">
         <v>0.5421276528180131</v>
       </c>
       <c r="V43">
-        <v>0.4677748335137318</v>
+        <v>0.4677748335137317</v>
       </c>
       <c r="W43">
         <v>0.4638385591830372</v>
@@ -6529,7 +6529,7 @@
         <v>0.6712510446948194</v>
       </c>
       <c r="R44">
-        <v>0.6260292273850719</v>
+        <v>0.6260292273850718</v>
       </c>
       <c r="S44">
         <v>0.5775851910434989</v>
@@ -6538,13 +6538,13 @@
         <v>0.5591988226510695</v>
       </c>
       <c r="U44">
-        <v>0.5774132969439264</v>
+        <v>0.5774132969439265</v>
       </c>
       <c r="V44">
         <v>0.5083332313890487</v>
       </c>
       <c r="W44">
-        <v>0.4937515928514591</v>
+        <v>0.4937515928514593</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -6597,10 +6597,10 @@
         <v>0.7149582657712805</v>
       </c>
       <c r="Q45">
-        <v>0.6696478738825816</v>
+        <v>0.6696478738825817</v>
       </c>
       <c r="R45">
-        <v>0.6551509495336435</v>
+        <v>0.6551509495336434</v>
       </c>
       <c r="S45">
         <v>0.5909102709393455</v>
@@ -6609,7 +6609,7 @@
         <v>0.5944311617965498</v>
       </c>
       <c r="U45">
-        <v>0.5963792541255821</v>
+        <v>0.596379254125582</v>
       </c>
       <c r="V45">
         <v>0.5251875575895789</v>
@@ -6677,7 +6677,7 @@
         <v>0.6314379329259888</v>
       </c>
       <c r="T46">
-        <v>0.6387617947427402</v>
+        <v>0.6387617947427403</v>
       </c>
       <c r="U46">
         <v>0.6321138083851513</v>
@@ -6686,7 +6686,7 @@
         <v>0.5658597484472347</v>
       </c>
       <c r="W46">
-        <v>0.5721998015096412</v>
+        <v>0.5721998015096413</v>
       </c>
     </row>
     <row r="47" spans="1:23">
@@ -6745,19 +6745,19 @@
         <v>0.7171552060578203</v>
       </c>
       <c r="S47">
-        <v>0.6878510759348595</v>
+        <v>0.6878510759348596</v>
       </c>
       <c r="T47">
         <v>0.6743013754736756</v>
       </c>
       <c r="U47">
-        <v>0.680724397528937</v>
+        <v>0.6807243975289371</v>
       </c>
       <c r="V47">
         <v>0.620067764211726</v>
       </c>
       <c r="W47">
-        <v>0.6177526642111127</v>
+        <v>0.6177526642111126</v>
       </c>
     </row>
     <row r="48" spans="1:23">
@@ -6825,7 +6825,7 @@
         <v>0.7253942272611545</v>
       </c>
       <c r="V48">
-        <v>0.6678579699899146</v>
+        <v>0.6678579699899148</v>
       </c>
       <c r="W48">
         <v>0.6579216442233343</v>
@@ -6866,7 +6866,7 @@
         <v>0.9317141099470206</v>
       </c>
       <c r="L49">
-        <v>0.8839588887378526</v>
+        <v>0.8839588887378527</v>
       </c>
       <c r="M49">
         <v>0.8529344488953738</v>
@@ -6884,7 +6884,7 @@
         <v>0.8205395766151308</v>
       </c>
       <c r="R49">
-        <v>0.8133293765025241</v>
+        <v>0.813329376502524</v>
       </c>
       <c r="S49">
         <v>0.7942330302441523</v>
@@ -6896,7 +6896,7 @@
         <v>0.7696237160849441</v>
       </c>
       <c r="V49">
-        <v>0.7445860710485952</v>
+        <v>0.7445860710485953</v>
       </c>
       <c r="W49">
         <v>0.7417909260102273</v>

</xml_diff>